<commit_message>
Added sound to Assest list.xlsx
</commit_message>
<xml_diff>
--- a/Assest list.xlsx
+++ b/Assest list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noah.cobb\Desktop\flatformer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian.erb\Desktop\flatformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>In progress</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>script damage per hit</t>
+  </si>
+  <si>
+    <t>Fly passive buzzing</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,35 +789,46 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B38" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>33</v>
       </c>
     </row>
@@ -983,18 +997,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1016,14 +1030,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
@@ -1037,4 +1043,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added rest of sprites
</commit_message>
<xml_diff>
--- a/Assest list.xlsx
+++ b/Assest list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezekiel.lacy\Desktop\flatformer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydan.long\Desktop\flatformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>In progress</t>
   </si>
@@ -159,18 +159,6 @@
     <t>Tree 1-3</t>
   </si>
   <si>
-    <t>Cload 1-3</t>
-  </si>
-  <si>
-    <t>Back ground mountain 1-2</t>
-  </si>
-  <si>
-    <t>flowers 1-6</t>
-  </si>
-  <si>
-    <t>Dummy</t>
-  </si>
-  <si>
     <t>Cart</t>
   </si>
   <si>
@@ -184,13 +172,37 @@
   </si>
   <si>
     <t>Windmill perpeller</t>
+  </si>
+  <si>
+    <t>Cloud 1-3</t>
+  </si>
+  <si>
+    <t>Small dummy</t>
+  </si>
+  <si>
+    <t>Back ground mountain 1-3</t>
+  </si>
+  <si>
+    <t>flowers 1-9</t>
+  </si>
+  <si>
+    <t>Dummy 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grass </t>
+  </si>
+  <si>
+    <t>Wagon</t>
+  </si>
+  <si>
+    <t>groung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +212,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -227,12 +247,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +634,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -624,7 +645,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>12</v>
@@ -671,7 +692,7 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -682,7 +703,7 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -692,7 +713,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -702,7 +723,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -712,7 +733,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -722,7 +743,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -732,7 +753,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -742,7 +763,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -752,7 +773,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -760,149 +781,179 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B44" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>29</v>
-      </c>
+      <c r="B46" s="1"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>30</v>
-      </c>
+      <c r="B47" s="1"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1071,18 +1122,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1104,14 +1155,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
@@ -1125,4 +1168,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sorted and simplified list
</commit_message>
<xml_diff>
--- a/Assest list.xlsx
+++ b/Assest list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aydan.long\Desktop\flatformer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christian.erb\Desktop\flatformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>In progress</t>
   </si>
@@ -36,21 +36,6 @@
     <t xml:space="preserve">Knight / Player </t>
   </si>
   <si>
-    <t xml:space="preserve">Script health </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Script </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sound </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprites </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prefabs </t>
-  </si>
-  <si>
     <t>Implemented</t>
   </si>
   <si>
@@ -72,130 +57,145 @@
     <t>Not Started/Assigned To</t>
   </si>
   <si>
-    <t xml:space="preserve">Script scene change </t>
-  </si>
-  <si>
     <t>Body</t>
   </si>
   <si>
     <t>Legs</t>
   </si>
   <si>
-    <t>Fly damage sound</t>
-  </si>
-  <si>
-    <t>Boss fly damage sound</t>
-  </si>
-  <si>
-    <t>Armor clink/Take damage/Menu button</t>
-  </si>
-  <si>
-    <t>In game music</t>
-  </si>
-  <si>
-    <t>Jump whoosh</t>
-  </si>
-  <si>
-    <t>Hitting dummy wooden click</t>
-  </si>
-  <si>
-    <t>Windmill creaking</t>
-  </si>
-  <si>
-    <t>Door open</t>
-  </si>
-  <si>
-    <t>Ambient sounds of start/end screen</t>
-  </si>
-  <si>
-    <t>Death oof</t>
-  </si>
-  <si>
-    <t>Small enemy</t>
-  </si>
-  <si>
-    <t>Large enemy</t>
-  </si>
-  <si>
-    <t>Enviromental objects</t>
-  </si>
-  <si>
-    <t>player</t>
-  </si>
-  <si>
-    <t>button</t>
-  </si>
-  <si>
-    <t>particle effects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">script scene change </t>
-  </si>
-  <si>
-    <t>script enemy movement</t>
-  </si>
-  <si>
-    <t>script player controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">script game over </t>
-  </si>
-  <si>
-    <t>script camera</t>
-  </si>
-  <si>
-    <t>script damage per hit</t>
-  </si>
-  <si>
-    <t>Fly passive buzzing</t>
-  </si>
-  <si>
-    <t>Fly</t>
-  </si>
-  <si>
-    <t>Fly wings</t>
-  </si>
-  <si>
-    <t>Tree 1-3</t>
-  </si>
-  <si>
-    <t>Cart</t>
-  </si>
-  <si>
-    <t>Bushes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Windmill </t>
-  </si>
-  <si>
-    <t>Door</t>
-  </si>
-  <si>
-    <t>Windmill perpeller</t>
-  </si>
-  <si>
-    <t>Cloud 1-3</t>
-  </si>
-  <si>
-    <t>Small dummy</t>
-  </si>
-  <si>
-    <t>Back ground mountain 1-3</t>
-  </si>
-  <si>
-    <t>flowers 1-9</t>
-  </si>
-  <si>
-    <t>Dummy 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grass </t>
-  </si>
-  <si>
-    <t>Wagon</t>
-  </si>
-  <si>
-    <t>groung</t>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>Sprites</t>
+  </si>
+  <si>
+    <t>Sounds</t>
+  </si>
+  <si>
+    <t>Whoosh</t>
+  </si>
+  <si>
+    <t>Armor clink</t>
+  </si>
+  <si>
+    <t>SoundKnightSwordSwing</t>
+  </si>
+  <si>
+    <t>SoundKnightDamaged</t>
+  </si>
+  <si>
+    <t>SoundKnightDead</t>
+  </si>
+  <si>
+    <t>SoundKnightJump</t>
+  </si>
+  <si>
+    <t>Scripts</t>
+  </si>
+  <si>
+    <t>ScriptKnightHealth</t>
+  </si>
+  <si>
+    <t>ScriptKnightPlayerController</t>
+  </si>
+  <si>
+    <t>ScriptKnightSword</t>
+  </si>
+  <si>
+    <t>Controls knight's health</t>
+  </si>
+  <si>
+    <t>Controls knight's movement</t>
+  </si>
+  <si>
+    <t>Controls sword rotation and damage</t>
+  </si>
+  <si>
+    <t>Scene</t>
+  </si>
+  <si>
+    <t>SpriteTree&lt;1-3&gt;</t>
+  </si>
+  <si>
+    <t>SpriteCloud&lt;1-3&gt;</t>
+  </si>
+  <si>
+    <t>SpriteMountain&lt;1-3&gt;</t>
+  </si>
+  <si>
+    <t>SpriteFlower&lt;1-9&gt;</t>
+  </si>
+  <si>
+    <t>SpriteCart</t>
+  </si>
+  <si>
+    <t>SpriteBushes</t>
+  </si>
+  <si>
+    <t>SpriteGround</t>
+  </si>
+  <si>
+    <t>SpriteWagon</t>
+  </si>
+  <si>
+    <t>SpriteGrass</t>
+  </si>
+  <si>
+    <t>SoundScreenMusic</t>
+  </si>
+  <si>
+    <t>SoundGameMusic</t>
+  </si>
+  <si>
+    <t>ScriptSceneChange</t>
+  </si>
+  <si>
+    <t>ScriptGameOver</t>
+  </si>
+  <si>
+    <t>ScriptCamera</t>
+  </si>
+  <si>
+    <t>Prefabs</t>
+  </si>
+  <si>
+    <t>PrefabKnight</t>
+  </si>
+  <si>
+    <t>Flies</t>
+  </si>
+  <si>
+    <t>SpriteFly</t>
+  </si>
+  <si>
+    <t>SoundFlyDamage</t>
+  </si>
+  <si>
+    <t>SoundFlyBuzz</t>
+  </si>
+  <si>
+    <t>ScriptFlyHealth</t>
+  </si>
+  <si>
+    <t>ScriptFlyController</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>SpriteDummy</t>
+  </si>
+  <si>
+    <t>SoundDummy</t>
+  </si>
+  <si>
+    <t>ScriptDummy</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -568,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,377 +584,384 @@
     <col min="6" max="6" width="26.28515625" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="37" customWidth="1"/>
+    <col min="9" max="10" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="B18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>46</v>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="1"/>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="D27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="D32" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="D35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="D43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D54" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1122,18 +1129,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1155,6 +1162,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
@@ -1168,12 +1183,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated name of a sound
</commit_message>
<xml_diff>
--- a/Assest list.xlsx
+++ b/Assest list.xlsx
@@ -141,9 +141,6 @@
     <t>SpriteGrass</t>
   </si>
   <si>
-    <t>SoundScreenMusic</t>
-  </si>
-  <si>
     <t>SoundGameMusic</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>SoundMainTheme</t>
   </si>
 </sst>
 </file>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,10 +598,10 @@
         <v>8</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -759,10 +759,10 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
         <v>42</v>
-      </c>
-      <c r="D17" t="s">
-        <v>43</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -845,13 +845,13 @@
         <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="D32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,19 +859,19 @@
         <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>
       <c r="C38" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,7 +892,7 @@
         <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -904,13 +904,13 @@
         <v>13</v>
       </c>
       <c r="D42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,13 +923,13 @@
         <v>20</v>
       </c>
       <c r="D45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="D46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -937,7 +937,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C48" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
@@ -945,7 +945,7 @@
         <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.25">
@@ -953,7 +953,7 @@
         <v>13</v>
       </c>
       <c r="D52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
         <v>20</v>
       </c>
       <c r="D54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1129,18 +1129,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1162,14 +1162,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
@@ -1183,4 +1175,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Missed sound, fixed it
</commit_message>
<xml_diff>
--- a/Assest list.xlsx
+++ b/Assest list.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
   <si>
     <t>In progress</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Nick</t>
+  </si>
+  <si>
+    <t>SoundAmbientBirds</t>
   </si>
 </sst>
 </file>
@@ -576,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,167 +800,172 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B68" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="B69" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1126,18 +1134,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1159,14 +1167,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
@@ -1180,4 +1180,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Signed off on completing audio
</commit_message>
<xml_diff>
--- a/Assest list.xlsx
+++ b/Assest list.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
   <si>
     <t>In progress</t>
   </si>
@@ -217,6 +217,33 @@
   </si>
   <si>
     <t>SoundAmbientBirds</t>
+  </si>
+  <si>
+    <t>ONCE ASSETS FIXED:</t>
+  </si>
+  <si>
+    <t>Nick 2:27</t>
+  </si>
+  <si>
+    <t>Begin working in sandbox</t>
+  </si>
+  <si>
+    <t>Implement files individually</t>
+  </si>
+  <si>
+    <t>Sounds:</t>
+  </si>
+  <si>
+    <t>Sprites:</t>
+  </si>
+  <si>
+    <t>Scripts:</t>
+  </si>
+  <si>
+    <t>ONCE ASSETS IMPLEMENTED:</t>
+  </si>
+  <si>
+    <t>Begin combining sandboxes</t>
   </si>
 </sst>
 </file>
@@ -579,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,6 +985,9 @@
       <c r="B69" t="s">
         <v>61</v>
       </c>
+      <c r="C69" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
@@ -967,6 +997,49 @@
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added people to asset list
</commit_message>
<xml_diff>
--- a/Assest list.xlsx
+++ b/Assest list.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>In progress</t>
   </si>
@@ -207,43 +207,16 @@
     <t>All Sounds</t>
   </si>
   <si>
-    <t>Scripts pt 1</t>
-  </si>
-  <si>
-    <t>Scripts pt 2</t>
-  </si>
-  <si>
     <t>Nick</t>
   </si>
   <si>
     <t>SoundAmbientBirds</t>
   </si>
   <si>
-    <t>ONCE ASSETS FIXED:</t>
-  </si>
-  <si>
-    <t>Nick 2:27</t>
-  </si>
-  <si>
-    <t>Begin working in sandbox</t>
-  </si>
-  <si>
-    <t>Implement files individually</t>
-  </si>
-  <si>
-    <t>Sounds:</t>
-  </si>
-  <si>
-    <t>Sprites:</t>
-  </si>
-  <si>
-    <t>Scripts:</t>
-  </si>
-  <si>
-    <t>ONCE ASSETS IMPLEMENTED:</t>
-  </si>
-  <si>
-    <t>Begin combining sandboxes</t>
+    <t>Ayden/Zeke</t>
+  </si>
+  <si>
+    <t>Noah</t>
   </si>
 </sst>
 </file>
@@ -609,7 +582,7 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +802,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -977,70 +950,82 @@
       <c r="A68" s="3" t="s">
         <v>57</v>
       </c>
+      <c r="B68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" t="s">
+        <v>61</v>
+      </c>
+      <c r="E68" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="D69" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>59</v>
+        <v>14</v>
+      </c>
+      <c r="B70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" t="s">
+        <v>62</v>
+      </c>
+      <c r="D70" t="s">
+        <v>62</v>
+      </c>
+      <c r="E70" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="A71" s="3"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="A73" s="3"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="A74" s="3"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="A75" s="3"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="A76" s="3"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
-        <v>68</v>
-      </c>
+      <c r="A77" s="3"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
-        <v>69</v>
-      </c>
+      <c r="A78" s="3"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="A80" s="3"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>71</v>
-      </c>
+      <c r="A81" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1207,18 +1192,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1240,6 +1225,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2515DB3B-AFD4-479F-850C-E15ACF9C8EE2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2c372ca1-4d00-4da0-9d60-1d24f5b7546b"/>
@@ -1253,12 +1246,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB2AA6DC-D7DC-43A1-8030-BE38C0100496}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>